<commit_message>
Update pension income modesl
-Introduce a separate model for pension income in the first period of retirement (I4a) and in subsequent periods (I4b).
</commit_message>
<xml_diff>
--- a/input/reg_RMSE.xlsx
+++ b/input/reg_RMSE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69606B91-95E7-4545-855B-5F17E5F057FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CDBBB2-83ED-476F-B3AA-74390B3869D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Date modified</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>S1b</t>
+  </si>
+  <si>
+    <t>I4a</t>
+  </si>
+  <si>
+    <t>I4b</t>
   </si>
 </sst>
 </file>
@@ -525,10 +531,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530F7AD6-02C1-41F5-9B11-F88D7B76E795}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,105 +616,121 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B10">
-        <v>0.66049632562288152</v>
+        <v>3.4780000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B11">
-        <v>0.62854363379376488</v>
+        <v>1.524</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>0.36533547999999999</v>
+        <v>0.66049632562288152</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>0.71279694000000005</v>
+        <v>0.62854363379376488</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>0.33935410999999999</v>
+        <v>0.36533547999999999</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>0.52967986</v>
+        <v>0.71279694000000005</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>1.528311</v>
+        <v>0.33935410999999999</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B17">
-        <v>1.1671</v>
+        <v>0.52967986</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18">
-        <v>1.2093</v>
+        <v>1.528311</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B19">
-        <v>0.98887999999999998</v>
+        <v>1.1671</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20">
-        <v>0.95128999999999997</v>
+        <v>1.2093</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>0.84714999999999996</v>
+        <v>0.98887999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>0.95128999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>0.84714999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B22">
+      <c r="B24">
         <v>0.94706000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update private pension income models
-This update distinguishes between probability of receiving private pension income and the level of income
-It also improves modelling of private pension income for individuals who are observed to be retired in the first year
</commit_message>
<xml_diff>
--- a/input/reg_RMSE.xlsx
+++ b/input/reg_RMSE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CDBBB2-83ED-476F-B3AA-74390B3869D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37114C62-1D3A-4B6C-9F31-95D76211C70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>Date modified</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>I4b</t>
+  </si>
+  <si>
+    <t>I5b</t>
+  </si>
+  <si>
+    <t>I6b</t>
   </si>
 </sst>
 </file>
@@ -531,10 +537,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530F7AD6-02C1-41F5-9B11-F88D7B76E795}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,105 +638,121 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B12">
-        <v>0.66049632562288152</v>
+        <v>1006.2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B13">
-        <v>0.62854363379376488</v>
+        <v>913.94</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>0.36533547999999999</v>
+        <v>0.66049632562288152</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>0.71279694000000005</v>
+        <v>0.62854363379376488</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>0.33935410999999999</v>
+        <v>0.36533547999999999</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>0.52967986</v>
+        <v>0.71279694000000005</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>1.528311</v>
+        <v>0.33935410999999999</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>1.1671</v>
+        <v>0.52967986</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>1.2093</v>
+        <v>1.528311</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B21">
-        <v>0.98887999999999998</v>
+        <v>1.1671</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>0.95128999999999997</v>
+        <v>1.2093</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>0.84714999999999996</v>
+        <v>0.98887999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>0.95128999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>0.84714999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B24">
+      <c r="B26">
         <v>0.94706000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
incomplete validation of new social care routines
</commit_message>
<xml_diff>
--- a/input/reg_RMSE.xlsx
+++ b/input/reg_RMSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9831F438-893B-4340-BE69-0CF96A653B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D592C26-6B28-4C2C-9420-C52C55C6839D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24360" yWindow="3165" windowWidth="19140" windowHeight="10245" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530F7AD6-02C1-41F5-9B11-F88D7B76E795}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,7 +734,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0.94706000000000001</v>
+        <v>0.94330000000000003</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -742,7 +742,7 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>1.2428999999999999</v>
+        <v>1.2788999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finalise uk update of data and parameters
</commit_message>
<xml_diff>
--- a/input/reg_RMSE.xlsx
+++ b/input/reg_RMSE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\temp\Daria current\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE69E4E-3FE6-4649-9E43-8ADC492F2FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6B8EE8-5FEA-48B5-A928-BEFFF950AA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="1755" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -109,7 +109,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -394,15 +395,15 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,39 +411,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>10.270364723275875</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <v>0.5511963385465366</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>23.729008366969978</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>0.56378226458419012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>14.165731818956298</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>0.3588496779494994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>25.876068646206658</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>0.37499140584966989</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -450,7 +451,7 @@
         <v>2.4158001968775116</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -458,7 +459,7 @@
         <v>1.8361431734912119</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -466,7 +467,7 @@
         <v>1.5969934128957666</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -474,7 +475,7 @@
         <v>884.81552442493353</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -482,7 +483,7 @@
         <v>4.4850000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -490,7 +491,7 @@
         <v>1.528311</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -498,7 +499,7 @@
         <v>1.1671</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -506,7 +507,7 @@
         <v>1.2093</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -514,7 +515,7 @@
         <v>0.98887999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -522,7 +523,7 @@
         <v>0.95128999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -530,7 +531,7 @@
         <v>0.84714999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -538,7 +539,7 @@
         <v>0.94330000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
check and confirm all input regression files
</commit_message>
<xml_diff>
--- a/input/reg_RMSE.xlsx
+++ b/input/reg_RMSE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17912E6E-338A-4E4A-80EB-90DC9675FDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFAB6AE-AF73-467E-82AA-7927A16E683F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Date modified</t>
   </si>
@@ -118,9 +118,6 @@
     <t>S1b</t>
   </si>
   <si>
-    <t>I4a</t>
-  </si>
-  <si>
     <t>I4b</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
   </si>
   <si>
     <t>I5b</t>
-  </si>
-  <si>
-    <t>I6b</t>
   </si>
 </sst>
 </file>
@@ -175,7 +169,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -185,6 +179,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,15 +535,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530F7AD6-02C1-41F5-9B11-F88D7B76E795}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B27"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -561,210 +556,138 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B2">
-        <v>0.74804999999999999</v>
+        <v>0.5511963385465366</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.76078000000000001</v>
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>0.56378226458419012</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>4.4850000000000003</v>
+        <v>0.3588496779494994</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B5">
-        <v>2.5001000000000002</v>
+        <v>0.37499140584966989</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1.3163</v>
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>2.4158001968775116</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7">
-        <v>1.9548000000000001</v>
+        <v>1.8361431734912119</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B8">
-        <v>1.6348</v>
+        <v>1.5969934128957666</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B9">
-        <v>0.31433</v>
+        <v>884.81552442493353</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10">
-        <v>3.4780000000000002</v>
+      <c r="A10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1.528311</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1.1671</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1.2093</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.98887999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0.95128999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.84714999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0.94330000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B11">
-        <v>1.524</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12">
-        <v>1006.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13">
-        <v>913.94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>0.66049632562288152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>0.62854363379376488</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>0.36533547999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>0.71279694000000005</v>
+      <c r="B17" s="5">
+        <v>1.2788999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B18">
-        <v>0.33935410999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>0.52967986</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>1.528311</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21">
-        <v>1.1671</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22">
-        <v>1.2093</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23">
-        <v>0.98887999999999998</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24">
-        <v>0.95128999999999997</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25">
-        <v>0.84714999999999996</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>0.94330000000000003</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27">
-        <v>1.2788999999999999</v>
+        <v>4.4850000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>